<commit_message>
update function check list: add User/ Common/ Report Other user
</commit_message>
<xml_diff>
--- a/WIP/Documents/Function check list.xlsx
+++ b/WIP/Documents/Function check list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project\WingS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_WingS\201609JS01\WIP\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
   <si>
     <t>Return Time</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>Change report's status</t>
+  </si>
+  <si>
+    <t>Report Other User</t>
   </si>
 </sst>
 </file>
@@ -249,7 +252,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -317,6 +320,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -496,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -517,8 +525,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -566,32 +572,17 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.249977111117893"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -792,13 +783,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="23"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="44"/>
         </left>
@@ -810,6 +794,34 @@
         </top>
         <bottom style="thin">
           <color indexed="44"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="23"/>
         </bottom>
       </border>
     </dxf>
@@ -929,14 +941,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:F55" totalsRowShown="0" headerRowDxfId="9" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
-  <autoFilter ref="B3:F55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:F56" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="B3:F56"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="No" dataDxfId="5"/>
-    <tableColumn id="2" name="Group" dataDxfId="4"/>
-    <tableColumn id="3" name="Function" dataDxfId="3"/>
-    <tableColumn id="4" name="Status" dataDxfId="2"/>
-    <tableColumn id="5" name="Return Time" dataDxfId="1"/>
+    <tableColumn id="1" name="No" dataDxfId="4"/>
+    <tableColumn id="2" name="Group" dataDxfId="3"/>
+    <tableColumn id="3" name="Function" dataDxfId="2"/>
+    <tableColumn id="4" name="Status" dataDxfId="1"/>
+    <tableColumn id="5" name="Return Time" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1231,10 +1243,10 @@
     <tabColor indexed="41"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:F55"/>
+  <dimension ref="B2:F56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" topLeftCell="A14" zoomScaleNormal="100" zoomScalePageLayoutView="86" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="86" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1249,10 +1261,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1267,7 +1279,7 @@
       <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -1275,620 +1287,631 @@
       </c>
     </row>
     <row r="4" spans="2:6" s="6" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="20"/>
-      <c r="C4" s="21" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="13">
+      <c r="B5" s="11">
         <v>1</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="13">
+      <c r="B6" s="11">
         <v>2</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="13">
+      <c r="B7" s="11">
         <v>3</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>4</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="13">
+      <c r="B9" s="11">
         <v>5</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="24"/>
-    </row>
-    <row r="10" spans="2:6" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="2:6" s="15" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
     </row>
     <row r="11" spans="2:6" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="27"/>
-      <c r="C11" s="21" t="s">
+      <c r="B11" s="25"/>
+      <c r="C11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="27"/>
     </row>
     <row r="12" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="13">
+      <c r="B12" s="11">
         <v>6</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="24"/>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="13">
+      <c r="B13" s="11">
         <v>7</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="13" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="24"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B14" s="13">
+      <c r="B14" s="11">
         <v>8</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="13" t="s">
+      <c r="C14" s="12"/>
+      <c r="D14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="24"/>
+      <c r="F14" s="22"/>
     </row>
     <row r="15" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="13">
+      <c r="B15" s="11">
         <v>9</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="13" t="s">
+      <c r="C15" s="12"/>
+      <c r="D15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="24"/>
+      <c r="F15" s="22"/>
     </row>
     <row r="16" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B16" s="13">
+      <c r="B16" s="11">
         <v>11</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="13" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="24"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="22"/>
     </row>
     <row r="17" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B17" s="13">
+      <c r="B17" s="11">
         <v>12</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="13" t="s">
+      <c r="C17" s="12"/>
+      <c r="D17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="24"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="22"/>
     </row>
     <row r="18" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B18" s="13">
+      <c r="B18" s="11">
         <v>13</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="13" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="24"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="22"/>
     </row>
     <row r="19" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B19" s="13">
+      <c r="B19" s="11">
         <v>14</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="13" t="s">
+      <c r="C19" s="12"/>
+      <c r="D19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="30"/>
-      <c r="F19" s="24"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="22"/>
     </row>
     <row r="20" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B20" s="13">
+      <c r="B20" s="11">
         <v>15</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="13" t="s">
+      <c r="C20" s="12"/>
+      <c r="D20" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="24"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="22"/>
     </row>
     <row r="21" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B21" s="13">
+      <c r="B21" s="11">
         <v>16</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="13" t="s">
+      <c r="C21" s="12"/>
+      <c r="D21" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="24"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B22" s="13">
+      <c r="B22" s="11">
         <v>17</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="13" t="s">
+      <c r="C22" s="13"/>
+      <c r="D22" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="24"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="22"/>
     </row>
     <row r="23" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B23" s="30">
+      <c r="B23" s="11">
         <v>18</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="37"/>
+      <c r="D23" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+    </row>
+    <row r="24" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="11">
+        <v>19</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D24" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E24" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="24"/>
-    </row>
-    <row r="24" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B24" s="13">
-        <v>19</v>
-      </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="13" t="s">
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B25" s="11">
+        <v>20</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="D25" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E25" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="24"/>
-    </row>
-    <row r="25" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B25" s="30">
-        <v>20</v>
-      </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="13" t="s">
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B26" s="11">
+        <v>21</v>
+      </c>
+      <c r="C26" s="28"/>
+      <c r="D26" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="24"/>
-    </row>
-    <row r="26" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B26" s="30">
-        <v>21</v>
-      </c>
-      <c r="C26" s="19" t="s">
+      <c r="E26" s="28"/>
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B27" s="11">
+        <v>22</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="D27" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="30"/>
-      <c r="F26" s="24"/>
-    </row>
-    <row r="27" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B27" s="13">
-        <v>22</v>
-      </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30" t="s">
+      <c r="E27" s="28"/>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B28" s="11">
+        <v>23</v>
+      </c>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="30"/>
-      <c r="F27" s="24"/>
-    </row>
-    <row r="28" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B28" s="30">
-        <v>23</v>
-      </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="13" t="s">
+      <c r="E28" s="28"/>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B29" s="11">
+        <v>24</v>
+      </c>
+      <c r="C29" s="28"/>
+      <c r="D29" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="30"/>
-      <c r="F28" s="24"/>
-    </row>
-    <row r="29" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B29" s="13">
-        <v>24</v>
-      </c>
-      <c r="C29" s="31" t="s">
+      <c r="E29" s="28"/>
+      <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B30" s="11">
+        <v>25</v>
+      </c>
+      <c r="C30" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D30" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-    </row>
-    <row r="30" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B30" s="30">
-        <v>25</v>
-      </c>
-      <c r="C30" s="31" t="s">
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B31" s="11">
+        <v>26</v>
+      </c>
+      <c r="C31" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D31" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="30" t="s">
+      <c r="E31" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="24"/>
-    </row>
-    <row r="31" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B31" s="30">
-        <v>26</v>
-      </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30" t="s">
+      <c r="F31" s="22"/>
+    </row>
+    <row r="32" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B32" s="11">
+        <v>27</v>
+      </c>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E32" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="24"/>
-    </row>
-    <row r="32" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B32" s="13">
-        <v>27</v>
-      </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30" t="s">
+      <c r="F32" s="22"/>
+    </row>
+    <row r="33" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="11">
+        <v>28</v>
+      </c>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="30" t="s">
+      <c r="E33" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="24"/>
-    </row>
-    <row r="33" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B33" s="30">
-        <v>28</v>
-      </c>
-      <c r="C33" s="31" t="s">
+      <c r="F33" s="22"/>
+    </row>
+    <row r="34" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B34" s="11">
+        <v>29</v>
+      </c>
+      <c r="C34" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D34" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="24"/>
-    </row>
-    <row r="34" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B34" s="13">
-        <v>29</v>
-      </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30" t="s">
+      <c r="E34" s="28"/>
+      <c r="F34" s="22"/>
+    </row>
+    <row r="35" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B35" s="11">
+        <v>30</v>
+      </c>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="E34" s="30"/>
-      <c r="F34" s="24"/>
-    </row>
-    <row r="35" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B35" s="30">
-        <v>30</v>
-      </c>
-      <c r="C35" s="31" t="s">
+      <c r="E35" s="28"/>
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B36" s="11">
+        <v>31</v>
+      </c>
+      <c r="C36" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D36" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="30"/>
-      <c r="F35" s="24"/>
-    </row>
-    <row r="36" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B36" s="30">
-        <v>31</v>
-      </c>
-      <c r="C36" s="31" t="s">
+      <c r="E36" s="28"/>
+      <c r="F36" s="22"/>
+    </row>
+    <row r="37" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B37" s="11">
+        <v>32</v>
+      </c>
+      <c r="C37" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="30" t="s">
+      <c r="D37" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="30"/>
-      <c r="F36" s="24"/>
-    </row>
-    <row r="37" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B37" s="13">
-        <v>32</v>
-      </c>
-      <c r="C37" s="31" t="s">
+      <c r="E37" s="28"/>
+      <c r="F37" s="22"/>
+    </row>
+    <row r="38" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B38" s="11">
+        <v>33</v>
+      </c>
+      <c r="C38" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D38" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="30"/>
-      <c r="F37" s="24"/>
-    </row>
-    <row r="38" spans="2:6" s="6" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="27"/>
-      <c r="C38" s="21" t="s">
+      <c r="E38" s="28"/>
+      <c r="F38" s="22"/>
+    </row>
+    <row r="39" spans="2:6" s="6" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="25"/>
+      <c r="C39" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="29"/>
-    </row>
-    <row r="39" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="30">
-        <v>33</v>
-      </c>
-      <c r="C39" s="31" t="s">
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="27"/>
+    </row>
+    <row r="40" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="28">
+        <v>34</v>
+      </c>
+      <c r="C40" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="33" t="s">
+      <c r="D40" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="30"/>
-      <c r="F39" s="24"/>
-    </row>
-    <row r="40" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="30">
-        <v>34</v>
-      </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="34" t="s">
+      <c r="E40" s="28"/>
+      <c r="F40" s="22"/>
+    </row>
+    <row r="41" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="28">
+        <v>35</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="30"/>
-      <c r="F40" s="24"/>
-    </row>
-    <row r="41" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="30">
-        <v>35</v>
-      </c>
-      <c r="C41" s="30"/>
-      <c r="D41" s="35" t="s">
+      <c r="E41" s="28"/>
+      <c r="F41" s="22"/>
+    </row>
+    <row r="42" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="28">
+        <v>36</v>
+      </c>
+      <c r="C42" s="28"/>
+      <c r="D42" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E41" s="30"/>
-      <c r="F41" s="24"/>
-    </row>
-    <row r="42" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B42" s="30">
-        <v>36</v>
-      </c>
-      <c r="C42" s="31" t="s">
+      <c r="E42" s="28"/>
+      <c r="F42" s="22"/>
+    </row>
+    <row r="43" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B43" s="28">
+        <v>37</v>
+      </c>
+      <c r="C43" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D42" s="30" t="s">
+      <c r="D43" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-    </row>
-    <row r="43" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B43" s="30">
-        <v>37</v>
-      </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30" t="s">
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+    </row>
+    <row r="44" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B44" s="28">
+        <v>38</v>
+      </c>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-    </row>
-    <row r="44" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B44" s="30">
-        <v>38</v>
-      </c>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30" t="s">
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+    </row>
+    <row r="45" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B45" s="28">
+        <v>39</v>
+      </c>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-    </row>
-    <row r="45" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B45" s="30">
-        <v>39</v>
-      </c>
-      <c r="C45" s="19" t="s">
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+    </row>
+    <row r="46" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B46" s="28">
+        <v>40</v>
+      </c>
+      <c r="C46" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="36" t="s">
+      <c r="D46" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-    </row>
-    <row r="46" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B46" s="30">
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B47" s="28">
         <v>41</v>
       </c>
-      <c r="C46" s="27"/>
-      <c r="D46" s="36" t="s">
+      <c r="C47" s="25"/>
+      <c r="D47" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-    </row>
-    <row r="47" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B47" s="30">
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+    </row>
+    <row r="48" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B48" s="28">
         <v>42</v>
       </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="36" t="s">
+      <c r="C48" s="25"/>
+      <c r="D48" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-    </row>
-    <row r="48" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B48" s="30">
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+    </row>
+    <row r="49" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B49" s="28">
         <v>43</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="C49" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D48" s="36" t="s">
+      <c r="D49" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-    </row>
-    <row r="49" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B49" s="30">
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+    </row>
+    <row r="50" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B50" s="28">
         <v>44</v>
       </c>
-      <c r="C49" s="30"/>
-      <c r="D49" s="36" t="s">
+      <c r="C50" s="28"/>
+      <c r="D50" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-    </row>
-    <row r="50" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B50" s="30">
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+    </row>
+    <row r="51" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B51" s="28">
         <v>45</v>
       </c>
-      <c r="C50" s="30"/>
-      <c r="D50" s="36" t="s">
+      <c r="C51" s="28"/>
+      <c r="D51" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-    </row>
-    <row r="51" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B51" s="30">
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+    </row>
+    <row r="52" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B52" s="28">
         <v>46</v>
       </c>
-      <c r="C51" s="31" t="s">
+      <c r="C52" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="D51" s="30"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-    </row>
-    <row r="52" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B52" s="30">
+      <c r="D52" s="28"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+    </row>
+    <row r="53" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B53" s="28">
         <v>47</v>
       </c>
-      <c r="C52" s="31" t="s">
+      <c r="C53" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="D52" s="30" t="s">
+      <c r="D53" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-    </row>
-    <row r="53" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B53" s="30">
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+    </row>
+    <row r="54" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B54" s="28">
         <v>48</v>
       </c>
-      <c r="C53" s="25"/>
-      <c r="D53" s="30" t="s">
+      <c r="C54" s="23"/>
+      <c r="D54" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-    </row>
-    <row r="54" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B54" s="30">
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+    </row>
+    <row r="55" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B55" s="28">
         <v>49</v>
       </c>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30" t="s">
+      <c r="C55" s="28"/>
+      <c r="D55" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-    </row>
-    <row r="55" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B55" s="32"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+    </row>
+    <row r="56" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B56" s="30"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
[Add] Multiple Pop-up chatbox
</commit_message>
<xml_diff>
--- a/WIP/Documents/Function check list.xlsx
+++ b/WIP/Documents/Function check list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_WingS\201609JS01\WIP\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WingS\201609JS01\201609JS01\WIP\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
   <si>
     <t>Return Time</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t>Report Other User</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Create Organization</t>
   </si>
 </sst>
 </file>
@@ -504,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -572,11 +578,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -941,8 +950,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:F56" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="B3:F56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:F58" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="B3:F58"/>
   <tableColumns count="5">
     <tableColumn id="1" name="No" dataDxfId="4"/>
     <tableColumn id="2" name="Group" dataDxfId="3"/>
@@ -1243,10 +1252,10 @@
     <tabColor indexed="41"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:F56"/>
+  <dimension ref="B2:F58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="86" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1261,10 +1270,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="36"/>
+      <c r="C2" s="38"/>
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1440,7 +1449,9 @@
       <c r="D16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="28"/>
+      <c r="E16" s="28" t="s">
+        <v>10</v>
+      </c>
       <c r="F16" s="22"/>
     </row>
     <row r="17" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
@@ -1473,7 +1484,9 @@
       <c r="D19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="28"/>
+      <c r="E19" s="28" t="s">
+        <v>10</v>
+      </c>
       <c r="F19" s="22"/>
     </row>
     <row r="20" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
@@ -1484,7 +1497,9 @@
       <c r="D20" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="28"/>
+      <c r="E20" s="28" t="s">
+        <v>10</v>
+      </c>
       <c r="F20" s="22"/>
     </row>
     <row r="21" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
@@ -1513,12 +1528,12 @@
       <c r="B23" s="11">
         <v>18</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37" t="s">
+      <c r="C23" s="35"/>
+      <c r="D23" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
     </row>
     <row r="24" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B24" s="11">
@@ -1699,219 +1714,239 @@
       <c r="F37" s="22"/>
     </row>
     <row r="38" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B38" s="11">
+      <c r="B38" s="39"/>
+      <c r="C38" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="36"/>
+    </row>
+    <row r="39" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B39" s="39"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+    </row>
+    <row r="40" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B40" s="11">
         <v>33</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="C40" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="28" t="s">
+      <c r="D40" s="28" t="s">
         <v>46</v>
-      </c>
-      <c r="E38" s="28"/>
-      <c r="F38" s="22"/>
-    </row>
-    <row r="39" spans="2:6" s="6" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="25"/>
-      <c r="C39" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="27"/>
-    </row>
-    <row r="40" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="28">
-        <v>34</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="31" t="s">
-        <v>50</v>
       </c>
       <c r="E40" s="28"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="28">
-        <v>35</v>
-      </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="22"/>
+    <row r="41" spans="2:6" s="6" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="25"/>
+      <c r="C41" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="27"/>
     </row>
     <row r="42" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B42" s="28">
-        <v>36</v>
-      </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="33" t="s">
-        <v>52</v>
+        <v>34</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="31" t="s">
+        <v>50</v>
       </c>
       <c r="E42" s="28"/>
       <c r="F42" s="22"/>
     </row>
-    <row r="43" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="28">
-        <v>37</v>
-      </c>
-      <c r="C43" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E43" s="22"/>
+        <v>35</v>
+      </c>
+      <c r="C43" s="28"/>
+      <c r="D43" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E43" s="28"/>
       <c r="F43" s="22"/>
     </row>
-    <row r="44" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B44" s="28">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C44" s="28"/>
-      <c r="D44" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" s="22"/>
+      <c r="D44" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44" s="28"/>
       <c r="F44" s="22"/>
     </row>
     <row r="45" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B45" s="28">
-        <v>39</v>
-      </c>
-      <c r="C45" s="28"/>
+        <v>37</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>55</v>
+      </c>
       <c r="D45" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" s="22"/>
     </row>
     <row r="46" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B46" s="28">
-        <v>40</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D46" s="34" t="s">
-        <v>60</v>
+        <v>38</v>
+      </c>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28" t="s">
+        <v>57</v>
       </c>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
     </row>
     <row r="47" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B47" s="28">
-        <v>41</v>
-      </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="34" t="s">
-        <v>61</v>
+        <v>39</v>
+      </c>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
     </row>
     <row r="48" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B48" s="28">
-        <v>42</v>
-      </c>
-      <c r="C48" s="25"/>
+        <v>40</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>59</v>
+      </c>
       <c r="D48" s="34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
     </row>
     <row r="49" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B49" s="28">
-        <v>43</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>63</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C49" s="25"/>
       <c r="D49" s="34" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
     </row>
     <row r="50" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B50" s="28">
-        <v>44</v>
-      </c>
-      <c r="C50" s="28"/>
+        <v>42</v>
+      </c>
+      <c r="C50" s="25"/>
       <c r="D50" s="34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
     </row>
     <row r="51" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B51" s="28">
-        <v>45</v>
-      </c>
-      <c r="C51" s="28"/>
+        <v>43</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>63</v>
+      </c>
       <c r="D51" s="34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="22"/>
     </row>
     <row r="52" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B52" s="28">
-        <v>46</v>
-      </c>
-      <c r="C52" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D52" s="28"/>
+        <v>44</v>
+      </c>
+      <c r="C52" s="28"/>
+      <c r="D52" s="34" t="s">
+        <v>65</v>
+      </c>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
     </row>
     <row r="53" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B53" s="28">
-        <v>47</v>
-      </c>
-      <c r="C53" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53" s="28" t="s">
-        <v>69</v>
+        <v>45</v>
+      </c>
+      <c r="C53" s="28"/>
+      <c r="D53" s="34" t="s">
+        <v>66</v>
       </c>
       <c r="E53" s="22"/>
       <c r="F53" s="22"/>
     </row>
     <row r="54" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B54" s="28">
-        <v>48</v>
-      </c>
-      <c r="C54" s="23"/>
-      <c r="D54" s="28" t="s">
-        <v>70</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D54" s="28"/>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
     </row>
     <row r="55" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B55" s="28">
-        <v>49</v>
-      </c>
-      <c r="C55" s="28"/>
+        <v>47</v>
+      </c>
+      <c r="C55" s="29" t="s">
+        <v>68</v>
+      </c>
       <c r="D55" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E55" s="22"/>
       <c r="F55" s="22"/>
     </row>
     <row r="56" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B56" s="30"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
+      <c r="B56" s="28">
+        <v>48</v>
+      </c>
+      <c r="C56" s="23"/>
+      <c r="D56" s="28" t="s">
+        <v>70</v>
+      </c>
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
+    </row>
+    <row r="57" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B57" s="28">
+        <v>49</v>
+      </c>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
+    </row>
+    <row r="58" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B58" s="30"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
update check list function
</commit_message>
<xml_diff>
--- a/WIP/Documents/Function check list.xlsx
+++ b/WIP/Documents/Function check list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WingS\201609JS01\201609JS01\WIP\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_WingS\201609JS01\WIP\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
   <si>
     <t>Return Time</t>
   </si>
@@ -248,6 +248,21 @@
   </si>
   <si>
     <t>Create Organization</t>
+  </si>
+  <si>
+    <t>View Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Organization </t>
+  </si>
+  <si>
+    <t>80% còn một số phần chưa bind data</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>90% : chưa delete được ảnh logo lưu trong thư mục</t>
   </si>
 </sst>
 </file>
@@ -258,7 +273,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -331,6 +346,13 @@
       <color theme="1" tint="0.249977111117893"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Trebuchet MS"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -370,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -506,11 +528,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="23"/>
+      </left>
+      <right style="thin">
+        <color indexed="23"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -582,16 +617,41 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.249977111117893"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -950,14 +1010,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:F58" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="B3:F58"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="No" dataDxfId="4"/>
-    <tableColumn id="2" name="Group" dataDxfId="3"/>
-    <tableColumn id="3" name="Function" dataDxfId="2"/>
-    <tableColumn id="4" name="Status" dataDxfId="1"/>
-    <tableColumn id="5" name="Return Time" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:G59" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="B3:G59"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="No" dataDxfId="5"/>
+    <tableColumn id="2" name="Group" dataDxfId="4"/>
+    <tableColumn id="3" name="Function" dataDxfId="3"/>
+    <tableColumn id="4" name="Status" dataDxfId="2"/>
+    <tableColumn id="5" name="Return Time" dataDxfId="1"/>
+    <tableColumn id="6" name="Note" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1252,10 +1313,10 @@
     <tabColor indexed="41"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:F58"/>
+  <dimension ref="B2:G59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="86" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="86" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1266,19 +1327,20 @@
     <col min="4" max="4" width="33.42578125" style="7" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" style="8" customWidth="1"/>
     <col min="6" max="6" width="24.140625" style="8" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="7"/>
+    <col min="7" max="7" width="46.5703125" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="37" t="s">
+    <row r="2" spans="2:7" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="38"/>
+      <c r="C2" s="39"/>
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="2:6" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1294,8 +1356,11 @@
       <c r="F3" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" s="6" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" s="6" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="18"/>
       <c r="C4" s="19" t="s">
         <v>5</v>
@@ -1303,8 +1368,9 @@
       <c r="D4" s="20"/>
       <c r="E4" s="21"/>
       <c r="F4" s="22"/>
-    </row>
-    <row r="5" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G4" s="40"/>
+    </row>
+    <row r="5" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B5" s="11">
         <v>1</v>
       </c>
@@ -1318,8 +1384,9 @@
         <v>10</v>
       </c>
       <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G5" s="40"/>
+    </row>
+    <row r="6" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B6" s="11">
         <v>2</v>
       </c>
@@ -1331,8 +1398,9 @@
         <v>10</v>
       </c>
       <c r="F6" s="22"/>
-    </row>
-    <row r="7" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G6" s="40"/>
+    </row>
+    <row r="7" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B7" s="11">
         <v>3</v>
       </c>
@@ -1344,8 +1412,9 @@
         <v>10</v>
       </c>
       <c r="F7" s="22"/>
-    </row>
-    <row r="8" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G7" s="40"/>
+    </row>
+    <row r="8" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B8" s="11">
         <v>4</v>
       </c>
@@ -1357,8 +1426,9 @@
         <v>10</v>
       </c>
       <c r="F8" s="22"/>
-    </row>
-    <row r="9" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G8" s="40"/>
+    </row>
+    <row r="9" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B9" s="11">
         <v>5</v>
       </c>
@@ -1370,15 +1440,17 @@
         <v>10</v>
       </c>
       <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="2:6" s="15" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G9" s="40"/>
+    </row>
+    <row r="10" spans="2:7" s="15" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="24"/>
-    </row>
-    <row r="11" spans="2:6" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="40"/>
+    </row>
+    <row r="11" spans="2:7" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="25"/>
       <c r="C11" s="19" t="s">
         <v>14</v>
@@ -1386,8 +1458,9 @@
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
       <c r="F11" s="27"/>
-    </row>
-    <row r="12" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G11" s="40"/>
+    </row>
+    <row r="12" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B12" s="11">
         <v>6</v>
       </c>
@@ -1401,8 +1474,9 @@
         <v>10</v>
       </c>
       <c r="F12" s="22"/>
-    </row>
-    <row r="13" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G12" s="40"/>
+    </row>
+    <row r="13" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1414,8 +1488,9 @@
         <v>10</v>
       </c>
       <c r="F13" s="22"/>
-    </row>
-    <row r="14" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G13" s="40"/>
+    </row>
+    <row r="14" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B14" s="11">
         <v>8</v>
       </c>
@@ -1427,8 +1502,9 @@
         <v>10</v>
       </c>
       <c r="F14" s="22"/>
-    </row>
-    <row r="15" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G14" s="40"/>
+    </row>
+    <row r="15" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B15" s="11">
         <v>9</v>
       </c>
@@ -1440,8 +1516,9 @@
         <v>10</v>
       </c>
       <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G15" s="40"/>
+    </row>
+    <row r="16" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
         <v>11</v>
       </c>
@@ -1453,8 +1530,9 @@
         <v>10</v>
       </c>
       <c r="F16" s="22"/>
-    </row>
-    <row r="17" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G16" s="40"/>
+    </row>
+    <row r="17" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B17" s="11">
         <v>12</v>
       </c>
@@ -1464,8 +1542,9 @@
       </c>
       <c r="E17" s="28"/>
       <c r="F17" s="22"/>
-    </row>
-    <row r="18" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G17" s="40"/>
+    </row>
+    <row r="18" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
         <v>13</v>
       </c>
@@ -1475,8 +1554,9 @@
       </c>
       <c r="E18" s="28"/>
       <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G18" s="40"/>
+    </row>
+    <row r="19" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B19" s="11">
         <v>14</v>
       </c>
@@ -1488,8 +1568,9 @@
         <v>10</v>
       </c>
       <c r="F19" s="22"/>
-    </row>
-    <row r="20" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G19" s="40"/>
+    </row>
+    <row r="20" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B20" s="11">
         <v>15</v>
       </c>
@@ -1501,8 +1582,9 @@
         <v>10</v>
       </c>
       <c r="F20" s="22"/>
-    </row>
-    <row r="21" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G20" s="40"/>
+    </row>
+    <row r="21" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B21" s="11">
         <v>16</v>
       </c>
@@ -1512,8 +1594,9 @@
       </c>
       <c r="E21" s="28"/>
       <c r="F21" s="22"/>
-    </row>
-    <row r="22" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G21" s="40"/>
+    </row>
+    <row r="22" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>17</v>
       </c>
@@ -1523,8 +1606,9 @@
       </c>
       <c r="E22" s="28"/>
       <c r="F22" s="22"/>
-    </row>
-    <row r="23" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G22" s="40"/>
+    </row>
+    <row r="23" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B23" s="11">
         <v>18</v>
       </c>
@@ -1534,8 +1618,9 @@
       </c>
       <c r="E23" s="36"/>
       <c r="F23" s="36"/>
-    </row>
-    <row r="24" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G23" s="40"/>
+    </row>
+    <row r="24" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B24" s="11">
         <v>19</v>
       </c>
@@ -1549,8 +1634,9 @@
         <v>53</v>
       </c>
       <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G24" s="40"/>
+    </row>
+    <row r="25" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B25" s="11">
         <v>20</v>
       </c>
@@ -1562,8 +1648,9 @@
         <v>10</v>
       </c>
       <c r="F25" s="22"/>
-    </row>
-    <row r="26" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G25" s="40"/>
+    </row>
+    <row r="26" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B26" s="11">
         <v>21</v>
       </c>
@@ -1573,8 +1660,9 @@
       </c>
       <c r="E26" s="28"/>
       <c r="F26" s="22"/>
-    </row>
-    <row r="27" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G26" s="40"/>
+    </row>
+    <row r="27" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B27" s="11">
         <v>22</v>
       </c>
@@ -1586,8 +1674,9 @@
       </c>
       <c r="E27" s="28"/>
       <c r="F27" s="22"/>
-    </row>
-    <row r="28" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G27" s="40"/>
+    </row>
+    <row r="28" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B28" s="11">
         <v>23</v>
       </c>
@@ -1597,8 +1686,9 @@
       </c>
       <c r="E28" s="28"/>
       <c r="F28" s="22"/>
-    </row>
-    <row r="29" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G28" s="40"/>
+    </row>
+    <row r="29" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B29" s="11">
         <v>24</v>
       </c>
@@ -1608,8 +1698,9 @@
       </c>
       <c r="E29" s="28"/>
       <c r="F29" s="22"/>
-    </row>
-    <row r="30" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G29" s="40"/>
+    </row>
+    <row r="30" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B30" s="11">
         <v>25</v>
       </c>
@@ -1621,8 +1712,9 @@
       </c>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
-    </row>
-    <row r="31" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G30" s="40"/>
+    </row>
+    <row r="31" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B31" s="11">
         <v>26</v>
       </c>
@@ -1636,8 +1728,9 @@
         <v>54</v>
       </c>
       <c r="F31" s="22"/>
-    </row>
-    <row r="32" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G31" s="40"/>
+    </row>
+    <row r="32" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B32" s="11">
         <v>27</v>
       </c>
@@ -1649,8 +1742,9 @@
         <v>54</v>
       </c>
       <c r="F32" s="22"/>
-    </row>
-    <row r="33" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G32" s="40"/>
+    </row>
+    <row r="33" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B33" s="11">
         <v>28</v>
       </c>
@@ -1662,8 +1756,9 @@
         <v>54</v>
       </c>
       <c r="F33" s="22"/>
-    </row>
-    <row r="34" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G33" s="40"/>
+    </row>
+    <row r="34" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B34" s="11">
         <v>29</v>
       </c>
@@ -1675,8 +1770,9 @@
       </c>
       <c r="E34" s="28"/>
       <c r="F34" s="22"/>
-    </row>
-    <row r="35" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G34" s="40"/>
+    </row>
+    <row r="35" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B35" s="11">
         <v>30</v>
       </c>
@@ -1686,8 +1782,9 @@
       </c>
       <c r="E35" s="28"/>
       <c r="F35" s="22"/>
-    </row>
-    <row r="36" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G35" s="40"/>
+    </row>
+    <row r="36" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B36" s="11">
         <v>31</v>
       </c>
@@ -1699,8 +1796,9 @@
       </c>
       <c r="E36" s="28"/>
       <c r="F36" s="22"/>
-    </row>
-    <row r="37" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="G36" s="40"/>
+    </row>
+    <row r="37" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="B37" s="11">
         <v>32</v>
       </c>
@@ -1712,9 +1810,10 @@
       </c>
       <c r="E37" s="28"/>
       <c r="F37" s="22"/>
-    </row>
-    <row r="38" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B38" s="39"/>
+      <c r="G37" s="40"/>
+    </row>
+    <row r="38" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B38" s="37"/>
       <c r="C38" s="35" t="s">
         <v>73</v>
       </c>
@@ -1725,228 +1824,265 @@
         <v>10</v>
       </c>
       <c r="F38" s="36"/>
-    </row>
-    <row r="39" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B39" s="39"/>
+      <c r="G38" s="40"/>
+    </row>
+    <row r="39" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B39" s="37"/>
       <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
+      <c r="D39" s="35" t="s">
+        <v>75</v>
+      </c>
       <c r="E39" s="36"/>
       <c r="F39" s="36"/>
-    </row>
-    <row r="40" spans="2:6" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B40" s="11">
+      <c r="G39" s="40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B40" s="37"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B41" s="11">
         <v>33</v>
       </c>
-      <c r="C40" s="29" t="s">
+      <c r="C41" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="28" t="s">
+      <c r="D41" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="28"/>
-      <c r="F40" s="22"/>
-    </row>
-    <row r="41" spans="2:6" s="6" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="25"/>
-      <c r="C41" s="19" t="s">
+      <c r="E41" s="28"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="40"/>
+    </row>
+    <row r="42" spans="2:7" s="6" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="25"/>
+      <c r="C42" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="27"/>
-    </row>
-    <row r="42" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="28">
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="40"/>
+    </row>
+    <row r="43" spans="2:7" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="28">
         <v>34</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C43" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="31" t="s">
+      <c r="D43" s="31" t="s">
         <v>50</v>
-      </c>
-      <c r="E42" s="28"/>
-      <c r="F42" s="22"/>
-    </row>
-    <row r="43" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="28">
-        <v>35</v>
-      </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="32" t="s">
-        <v>51</v>
       </c>
       <c r="E43" s="28"/>
       <c r="F43" s="22"/>
-    </row>
-    <row r="44" spans="2:6" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G43" s="40"/>
+    </row>
+    <row r="44" spans="2:7" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B44" s="28">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C44" s="28"/>
-      <c r="D44" s="33" t="s">
-        <v>52</v>
+      <c r="D44" s="32" t="s">
+        <v>51</v>
       </c>
       <c r="E44" s="28"/>
       <c r="F44" s="22"/>
-    </row>
-    <row r="45" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="G44" s="40"/>
+    </row>
+    <row r="45" spans="2:7" s="6" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B45" s="28">
+        <v>36</v>
+      </c>
+      <c r="C45" s="28"/>
+      <c r="D45" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="28"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="40"/>
+    </row>
+    <row r="46" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B46" s="28">
         <v>37</v>
       </c>
-      <c r="C45" s="29" t="s">
+      <c r="C46" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D45" s="28" t="s">
+      <c r="D46" s="28" t="s">
         <v>56</v>
-      </c>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-    </row>
-    <row r="46" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B46" s="28">
-        <v>38</v>
-      </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28" t="s">
-        <v>57</v>
       </c>
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
-    </row>
-    <row r="47" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="G46" s="40"/>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B47" s="28">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C47" s="28"/>
       <c r="D47" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
-    </row>
-    <row r="48" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="G47" s="40"/>
+    </row>
+    <row r="48" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B48" s="28">
-        <v>40</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D48" s="34" t="s">
-        <v>60</v>
+        <v>39</v>
+      </c>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
-    </row>
-    <row r="49" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="G48" s="40"/>
+    </row>
+    <row r="49" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B49" s="28">
-        <v>41</v>
-      </c>
-      <c r="C49" s="25"/>
+        <v>40</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>59</v>
+      </c>
       <c r="D49" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
-    </row>
-    <row r="50" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="G49" s="40"/>
+    </row>
+    <row r="50" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B50" s="28">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C50" s="25"/>
       <c r="D50" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
-    </row>
-    <row r="51" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="G50" s="40"/>
+    </row>
+    <row r="51" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B51" s="28">
-        <v>43</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>63</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C51" s="25"/>
       <c r="D51" s="34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="22"/>
-    </row>
-    <row r="52" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="G51" s="40"/>
+    </row>
+    <row r="52" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B52" s="28">
-        <v>44</v>
-      </c>
-      <c r="C52" s="28"/>
+        <v>43</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>63</v>
+      </c>
       <c r="D52" s="34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
-    </row>
-    <row r="53" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="G52" s="40"/>
+    </row>
+    <row r="53" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B53" s="28">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C53" s="28"/>
       <c r="D53" s="34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E53" s="22"/>
       <c r="F53" s="22"/>
-    </row>
-    <row r="54" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="G53" s="40"/>
+    </row>
+    <row r="54" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B54" s="28">
-        <v>46</v>
-      </c>
-      <c r="C54" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D54" s="28"/>
+        <v>45</v>
+      </c>
+      <c r="C54" s="28"/>
+      <c r="D54" s="34" t="s">
+        <v>66</v>
+      </c>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
-    </row>
-    <row r="55" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="G54" s="40"/>
+    </row>
+    <row r="55" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B55" s="28">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D55" s="28" t="s">
-        <v>69</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D55" s="28"/>
       <c r="E55" s="22"/>
       <c r="F55" s="22"/>
-    </row>
-    <row r="56" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="G55" s="40"/>
+    </row>
+    <row r="56" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B56" s="28">
-        <v>48</v>
-      </c>
-      <c r="C56" s="23"/>
+        <v>47</v>
+      </c>
+      <c r="C56" s="29" t="s">
+        <v>68</v>
+      </c>
       <c r="D56" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E56" s="22"/>
       <c r="F56" s="22"/>
-    </row>
-    <row r="57" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="G56" s="40"/>
+    </row>
+    <row r="57" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B57" s="28">
-        <v>49</v>
-      </c>
-      <c r="C57" s="28"/>
+        <v>48</v>
+      </c>
+      <c r="C57" s="23"/>
       <c r="D57" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E57" s="22"/>
       <c r="F57" s="22"/>
-    </row>
-    <row r="58" spans="2:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B58" s="30"/>
+      <c r="G57" s="40"/>
+    </row>
+    <row r="58" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B58" s="28">
+        <v>49</v>
+      </c>
       <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
+      <c r="D58" s="28" t="s">
+        <v>71</v>
+      </c>
       <c r="E58" s="22"/>
       <c r="F58" s="22"/>
+      <c r="G58" s="40"/>
+    </row>
+    <row r="59" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B59" s="30"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>